<commit_message>
Added Mallet. Done thesis
</commit_message>
<xml_diff>
--- a/entities-count.xlsx
+++ b/entities-count.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\Anul 4\Licenta\licenta-ner\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="8250" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
   <si>
     <t>TIME</t>
   </si>
@@ -62,9 +67,6 @@
   </si>
   <si>
     <t>\\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t>Total</t>
@@ -73,8 +75,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,12 +126,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -164,7 +184,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -173,9 +195,25 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
             <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -274,13 +312,20 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
           <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -292,7 +337,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -312,7 +367,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -321,8 +378,25 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -370,8 +444,23 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -416,7 +505,13 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -424,8 +519,11 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -548,7 +646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,9 +678,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,6 +713,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -789,19 +889,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +909,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -817,7 +917,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -825,7 +925,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -833,7 +933,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -841,7 +941,7 @@
         <v>2549</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -849,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -857,7 +957,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -865,7 +965,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -873,7 +973,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -881,7 +981,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -889,7 +989,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -897,7 +997,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -905,7 +1005,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="1048576" spans="2:2">
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1048576">
         <f>SUM(B1:B1048575)</f>
         <v>11494</v>
@@ -913,262 +1013,267 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1">
+        <v>3089</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>2549</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1988</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1007</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>912</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>561</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>381</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>355</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>248</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>237</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>73</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C1:C13)</f>
+        <v>11494</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C14">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D2:D12" r:id="rId2" display="\\"/>
+    <hyperlink ref="D11" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1">
-        <v>3089</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>2549</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>1988</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>1007</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>912</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>561</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>381</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>355</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>248</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>237</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>73</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14">
-        <f>SUM(C1:C13)</f>
-        <v>11494</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="C1:C13">
-    <sortCondition descending="1" ref="C1"/>
-  </sortState>
-  <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1"/>
-    <hyperlink ref="D2:D12" r:id="rId2" display="\\"/>
-    <hyperlink ref="D13" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1">
-        <v>2549</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="B2">
         <v>1007</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1281,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1195,20 +1300,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1250,7 +1355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1264,9 +1369,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>

</xml_diff>